<commit_message>
Dados do mês de abril24
</commit_message>
<xml_diff>
--- a/bcw-operation-calendar.xlsx
+++ b/bcw-operation-calendar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis PC\Desktop\Projetos\BCW-AttendanceAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis PC\Desktop\Projetos\BCW-Queue-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8508F276-E7F5-4056-977C-04B33238FD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1771905-893F-4D8A-9D25-803A0EA1C0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4425" windowWidth="20730" windowHeight="11160" xr2:uid="{CB0BBA59-65E6-49DE-A584-2A9B09E573BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB0BBA59-65E6-49DE-A584-2A9B09E573BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -289,11 +289,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,8 +613,8 @@
   <dimension ref="A1:X923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A457" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A457" sqref="A457"/>
+      <pane ySplit="1" topLeftCell="A454" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G479" sqref="G479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20335,7 +20337,13 @@
         <v>51</v>
       </c>
       <c r="C458" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D458" s="2">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E458" s="2">
+        <v>0.79166666666666696</v>
       </c>
       <c r="I458" t="s">
         <v>64</v>
@@ -20457,7 +20465,13 @@
         <v>51</v>
       </c>
       <c r="C465" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D465" s="2">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E465" s="2">
+        <v>0.79166666666666696</v>
       </c>
       <c r="I465" t="s">
         <v>64</v>
@@ -20579,7 +20593,13 @@
         <v>51</v>
       </c>
       <c r="C472" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D472" s="2">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E472" s="2">
+        <v>0.79166666666666696</v>
       </c>
       <c r="I472" t="s">
         <v>64</v>
@@ -20707,7 +20727,13 @@
         <v>51</v>
       </c>
       <c r="C479" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D479" s="2">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E479" s="2">
+        <v>0.79166666666666696</v>
       </c>
       <c r="I479" t="s">
         <v>64</v>
@@ -20831,8 +20857,14 @@
       <c r="B486" t="s">
         <v>51</v>
       </c>
-      <c r="C486" t="s">
-        <v>14</v>
+      <c r="C486" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D486" s="5">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E486" s="5">
+        <v>0.79166666666666696</v>
       </c>
       <c r="I486" t="s">
         <v>64</v>

</xml_diff>